<commit_message>
Updating UC3 KPI description
</commit_message>
<xml_diff>
--- a/UC3_KPIs.xlsx
+++ b/UC3_KPIs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29728"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10208"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mefgovit.sharepoint.com/sites/glaciation/Documenti condivisi/General/7. Work Package 7 - Validation and Use cases/T7.3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/D064573/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1952" documentId="8_{562391A9-04D5-4E79-9277-07DD3D7E73E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D18E879-2F0B-45F8-9FD9-F57711B3550F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{002271A5-DB04-E047-AA58-4F322F1585A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="2" xr2:uid="{A98C65B7-165D-41E1-953F-98ED71E7C7A2}"/>
+    <workbookView xWindow="13260" yWindow="620" windowWidth="42800" windowHeight="22420" firstSheet="2" activeTab="2" xr2:uid="{A98C65B7-165D-41E1-953F-98ED71E7C7A2}"/>
   </bookViews>
   <sheets>
     <sheet name="From Proposal" sheetId="3" r:id="rId1"/>
@@ -37,26 +37,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>tc={2177C8FB-A941-4F7F-918D-0230B79E0F5D}</author>
-  </authors>
-  <commentList>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{2177C8FB-A941-4F7F-918D-0230B79E0F5D}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    It would be great if there was a KPI that the existence of GLACIATION improves the KPI for UC3</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="343">
   <si>
     <t>WP7 Objectives</t>
   </si>
@@ -1101,9 +1083,6 @@
     <t>Security and Compliance</t>
   </si>
   <si>
-    <t>//for consistency, took category name from UC2</t>
-  </si>
-  <si>
     <t>Privacy &amp; security guarantees</t>
   </si>
   <si>
@@ -1119,9 +1098,6 @@
     <t>Bit security level, epsilon privacy level</t>
   </si>
   <si>
-    <t>high security/privacy supported (PETS = Privacy-enhancing technologies, MPC = secure multi-party computation, DP = differential privacy)</t>
-  </si>
-  <si>
     <t>Parameterization of PETs</t>
   </si>
   <si>
@@ -1134,9 +1110,6 @@
     <t>Validate that PET implementations accept ranges</t>
   </si>
   <si>
-    <t>flexible parameters (e.g., also lower to medium security/privacy supported to gain efficiency, or less precision/accuracy to gain efficiency)</t>
-  </si>
-  <si>
     <t>Operational Efficiency</t>
   </si>
   <si>
@@ -1155,63 +1128,21 @@
     <t>E.g., accuracy, F1 score, MCC</t>
   </si>
   <si>
-    <t>See also slides from GA 2024-10: https://mefgovit.sharepoint.com/:p:/r/sites/glaciation/_layouts/15/Doc.aspx?sourcedoc=%7BB4D82FCB-9BFC-4CCD-8311-0EA0ECA1D89A%7D&amp;file=GLACIATION_GA_October_24_MASTER.pptx&amp;action=edit&amp;mobileredirect=true</t>
-  </si>
-  <si>
     <t>Reduced waste</t>
   </si>
   <si>
     <t>Reduce cost associated with waste or machine failure driven by improved prediction accuracy</t>
   </si>
   <si>
-    <t>5% less</t>
-  </si>
-  <si>
     <t>Approximate cost reduction from accuracy improvement</t>
   </si>
   <si>
     <t>(estimated) Dollar cost</t>
   </si>
   <si>
-    <t>Cost estimates via "Economics of Manufacturing Machinery Maintenance NIST 2016"</t>
-  </si>
-  <si>
     <t>Usability</t>
   </si>
   <si>
-    <t>//for consistency, maybe merge with "Visualization &amp; Reporting" from UC2? E.g., "Usability, Visualization &amp; Reporting"?</t>
-  </si>
-  <si>
-    <t>DP: visualize mechanisms</t>
-  </si>
-  <si>
-    <t>Provide visual feedback for DP parameterization, accuracy-privacy trade-off</t>
-  </si>
-  <si>
-    <t>Support at least 3 DP mechanisms and flexible parameter ranges</t>
-  </si>
-  <si>
-    <t>Number of functioning, provided mechanisms</t>
-  </si>
-  <si>
-    <t>Count of mechanisms</t>
-  </si>
-  <si>
-    <t>DP-Viz already ensures this</t>
-  </si>
-  <si>
-    <t>//DP: Multi-session support</t>
-  </si>
-  <si>
-    <t>//Run multiple sessions concurrently in one browser</t>
-  </si>
-  <si>
-    <t>//Support at least 3 sessions</t>
-  </si>
-  <si>
-    <t>Why crossed-out? Not longer guaranteed as DP-Viz developer changed position internally and is not available</t>
-  </si>
-  <si>
     <t>MPC: performant demo</t>
   </si>
   <si>
@@ -1230,9 +1161,6 @@
     <t>AI/ML Predictive Analytics KPIs</t>
   </si>
   <si>
-    <t>//for consistency, took category name from UC2 (more precise would be "Collaborative Prediction / Analytics")</t>
-  </si>
-  <si>
     <t>Training Time</t>
   </si>
   <si>
@@ -1248,9 +1176,6 @@
     <t>Seconds (or Minutes)</t>
   </si>
   <si>
-    <t xml:space="preserve">For concept evaluation, consider focusing on MP-SPDZ only (MPC engine in CarbyneStack instead of entire stack) </t>
-  </si>
-  <si>
     <t>Inference Time</t>
   </si>
   <si>
@@ -1281,56 +1206,62 @@
     <t>Business Reliability &amp; Deployability</t>
   </si>
   <si>
-    <t>//for consistency, took category name from UC1 (but added "&amp; Deployability")</t>
-  </si>
-  <si>
-    <t>SAP BTP Deployability</t>
-  </si>
-  <si>
-    <t>Succesful computation service deployment on SAP BTP</t>
-  </si>
-  <si>
     <t>Semi-automatic BTP deployment via SAP Gardener</t>
   </si>
   <si>
     <t>Successful deployment</t>
   </si>
   <si>
-    <t>Binary (yes/no) or qualitatively (e.g., ease of use, few clicks)</t>
-  </si>
-  <si>
     <t>Energy Efficiency</t>
   </si>
   <si>
-    <t>//potential KPI to showcase UC3 benefitting from Glaciation - only if we get MPC engine to run in Glaciation cluster</t>
-  </si>
-  <si>
-    <t>Added observability for energy efficiency</t>
-  </si>
-  <si>
     <t>leverage Glaciation services for measurements and observability</t>
   </si>
   <si>
     <t>observe additional, energy-related metrics (not measured by existing MPC/DP frameworks)</t>
   </si>
   <si>
-    <t>Glaciation provided, e.g., total power consumption, CPU utilization?</t>
-  </si>
-  <si>
-    <t>e.g., kWh, utilization percentage?</t>
-  </si>
-  <si>
-    <t>Cannot promise to actually manage to deploy MPC in Glaciation pods (ideally, multi-cluster setting, one MPC instance per cluster); could consider to deploy MPC/MP-SPDZ engine in (single-cluster) Glaciation setup just as possibility</t>
-  </si>
-  <si>
-    <t>NOTE: Concept Evaluation KPIS highlighted in light green like this</t>
+    <t>Glaciation provided, e.g., total power consumption, CPU utilization</t>
+  </si>
+  <si>
+    <t>Glaciation measurement unit</t>
+  </si>
+  <si>
+    <t>2% less</t>
+  </si>
+  <si>
+    <t>Succesful computation service deployment in business application context</t>
+  </si>
+  <si>
+    <t>Deployable in business application context</t>
+  </si>
+  <si>
+    <t>Observability for energy efficiency</t>
+  </si>
+  <si>
+    <t>Relative ease of use, i.e., usability </t>
+  </si>
+  <si>
+    <t>Hide technological complexities as much as possible</t>
+  </si>
+  <si>
+    <t>By providing more user-friendly abstractions for mostly command-line tools</t>
+  </si>
+  <si>
+    <t>Demonstrator, REST interfaces</t>
+  </si>
+  <si>
+    <t>Qualitiative: demonstrator, interfaces</t>
+  </si>
+  <si>
+    <t>Qualitative: feasable, simple setup</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1436,14 +1367,6 @@
       <family val="2"/>
     </font>
     <font>
-      <strike/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -1452,14 +1375,6 @@
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.499984740745262"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFC00000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1485,8 +1400,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1507,19 +1429,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1721,7 +1637,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1807,41 +1723,32 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1883,12 +1790,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName="OMahony, Aidan" id="{22644DE0-97B5-4F52-B8C7-D899A5CBF171}" userId="S::Aidan.Omahony@dell.com::d5b2573e-3cb8-4c23-9dc2-a764eba646db" providerId="AD"/>
-</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2206,14 +2107,6 @@
 </a:theme>
 </file>
 
-<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
-<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="B1" dT="2025-02-06T09:46:15.83" personId="{22644DE0-97B5-4F52-B8C7-D899A5CBF171}" id="{2177C8FB-A941-4F7F-918D-0230B79E0F5D}">
-    <text>It would be great if there was a KPI that the existence of GLACIATION improves the KPI for UC3</text>
-  </threadedComment>
-</ThreadedComments>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E9F3671-6D99-40E2-B04F-8FCE2D23BCED}">
   <dimension ref="A2:F93"/>
@@ -2222,67 +2115,67 @@
       <selection activeCell="C71" sqref="C71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.85546875" customWidth="1"/>
-    <col min="2" max="2" width="8.5703125" customWidth="1"/>
-    <col min="3" max="3" width="27.5703125" customWidth="1"/>
-    <col min="4" max="4" width="28.42578125" customWidth="1"/>
-    <col min="5" max="5" width="30.7109375" customWidth="1"/>
-    <col min="6" max="6" width="44.140625" customWidth="1"/>
+    <col min="1" max="1" width="7.83203125" customWidth="1"/>
+    <col min="2" max="2" width="8.5" customWidth="1"/>
+    <col min="3" max="3" width="27.5" customWidth="1"/>
+    <col min="4" max="4" width="28.5" customWidth="1"/>
+    <col min="5" max="5" width="30.6640625" customWidth="1"/>
+    <col min="6" max="6" width="44.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" ht="14.45" customHeight="1">
-      <c r="C2" s="44" t="s">
+    <row r="2" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C2" s="41" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="14.45" customHeight="1">
-      <c r="C3" s="44"/>
-    </row>
-    <row r="4" spans="1:6" ht="22.5" customHeight="1">
-      <c r="C4" s="45" t="s">
+    <row r="3" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C3" s="41"/>
+    </row>
+    <row r="4" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C4" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-    </row>
-    <row r="5" spans="1:6" ht="23.25" customHeight="1">
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-    </row>
-    <row r="6" spans="1:6" ht="23.25" customHeight="1">
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="45"/>
-    </row>
-    <row r="7" spans="1:6" ht="23.25" customHeight="1">
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+    </row>
+    <row r="5" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+    </row>
+    <row r="6" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="42"/>
+    </row>
+    <row r="7" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="10" spans="1:6" ht="15.6">
+    <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="32.25" customHeight="1">
+    <row r="12" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="45" t="s">
+      <c r="C12" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="45"/>
-      <c r="E12" s="45"/>
-      <c r="F12" s="45"/>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>5</v>
       </c>
@@ -2290,7 +2183,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>7</v>
       </c>
@@ -2298,24 +2191,24 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="45" t="s">
+      <c r="C16" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="45"/>
-      <c r="E16" s="45"/>
-      <c r="F16" s="45"/>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="C17" s="45"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="45"/>
-    </row>
-    <row r="18" spans="1:6">
+      <c r="D16" s="42"/>
+      <c r="E16" s="42"/>
+      <c r="F16" s="42"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C17" s="42"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="42"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>11</v>
       </c>
@@ -2323,7 +2216,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>13</v>
       </c>
@@ -2331,7 +2224,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>15</v>
       </c>
@@ -2340,7 +2233,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>17</v>
       </c>
@@ -2348,7 +2241,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>19</v>
       </c>
@@ -2356,7 +2249,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>21</v>
       </c>
@@ -2365,7 +2258,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>23</v>
       </c>
@@ -2373,7 +2266,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>25</v>
       </c>
@@ -2381,7 +2274,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>27</v>
       </c>
@@ -2389,7 +2282,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>29</v>
       </c>
@@ -2398,7 +2291,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>31</v>
       </c>
@@ -2406,7 +2299,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>33</v>
       </c>
@@ -2414,25 +2307,25 @@
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B34" s="2"/>
-      <c r="C34" s="45" t="s">
+      <c r="C34" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="D34" s="45"/>
-      <c r="E34" s="45"/>
-      <c r="F34" s="45"/>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="C35" s="45"/>
-      <c r="D35" s="45"/>
-      <c r="E35" s="45"/>
-      <c r="F35" s="45"/>
-    </row>
-    <row r="36" spans="1:6">
+      <c r="D34" s="42"/>
+      <c r="E34" s="42"/>
+      <c r="F34" s="42"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C35" s="42"/>
+      <c r="D35" s="42"/>
+      <c r="E35" s="42"/>
+      <c r="F35" s="42"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>37</v>
       </c>
@@ -2440,7 +2333,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
         <v>39</v>
       </c>
@@ -2448,7 +2341,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>41</v>
       </c>
@@ -2457,7 +2350,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
         <v>43</v>
       </c>
@@ -2465,7 +2358,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
         <v>45</v>
       </c>
@@ -2473,7 +2366,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
         <v>47</v>
       </c>
@@ -2481,7 +2374,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>49</v>
       </c>
@@ -2490,7 +2383,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
         <v>51</v>
       </c>
@@ -2501,7 +2394,7 @@
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
         <v>53</v>
       </c>
@@ -2512,54 +2405,54 @@
       <c r="E46" s="4"/>
       <c r="F46" s="4"/>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
         <v>55</v>
       </c>
-      <c r="C47" s="46" t="s">
+      <c r="C47" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="D47" s="46"/>
-      <c r="E47" s="46"/>
-      <c r="F47" s="46"/>
-    </row>
-    <row r="48" spans="1:6">
-      <c r="C48" s="46"/>
-      <c r="D48" s="46"/>
-      <c r="E48" s="46"/>
-      <c r="F48" s="46"/>
-    </row>
-    <row r="49" spans="1:6">
+      <c r="D47" s="43"/>
+      <c r="E47" s="43"/>
+      <c r="F47" s="43"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C48" s="43"/>
+      <c r="D48" s="43"/>
+      <c r="E48" s="43"/>
+      <c r="F48" s="43"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>57</v>
       </c>
       <c r="B50" s="2"/>
-      <c r="C50" s="45" t="s">
+      <c r="C50" s="42" t="s">
         <v>58</v>
       </c>
-      <c r="D50" s="45"/>
-      <c r="E50" s="45"/>
-      <c r="F50" s="45"/>
-    </row>
-    <row r="51" spans="1:6">
-      <c r="C51" s="45"/>
-      <c r="D51" s="45"/>
-      <c r="E51" s="45"/>
-      <c r="F51" s="45"/>
-    </row>
-    <row r="52" spans="1:6">
-      <c r="C52" s="45"/>
-      <c r="D52" s="45"/>
-      <c r="E52" s="45"/>
-      <c r="F52" s="45"/>
-    </row>
-    <row r="53" spans="1:6">
+      <c r="D50" s="42"/>
+      <c r="E50" s="42"/>
+      <c r="F50" s="42"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C51" s="42"/>
+      <c r="D51" s="42"/>
+      <c r="E51" s="42"/>
+      <c r="F51" s="42"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C52" s="42"/>
+      <c r="D52" s="42"/>
+      <c r="E52" s="42"/>
+      <c r="F52" s="42"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
         <v>59</v>
       </c>
@@ -2567,7 +2460,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
         <v>61</v>
       </c>
@@ -2575,37 +2468,37 @@
         <v>62</v>
       </c>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="58" spans="1:6">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B58" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="59" spans="1:6">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="61" spans="1:6">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="64" spans="1:6">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B65" t="s">
         <v>69</v>
       </c>
@@ -2613,17 +2506,17 @@
         <v>70</v>
       </c>
     </row>
-    <row r="66" spans="1:3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C66" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="67" spans="1:3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C67" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="68" spans="1:3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B68" t="s">
         <v>73</v>
       </c>
@@ -2631,17 +2524,17 @@
         <v>74</v>
       </c>
     </row>
-    <row r="69" spans="1:3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C69" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="70" spans="1:3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C70" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="71" spans="1:3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B71" t="s">
         <v>77</v>
       </c>
@@ -2649,12 +2542,12 @@
         <v>78</v>
       </c>
     </row>
-    <row r="72" spans="1:3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C72" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="74" spans="1:3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B74" t="s">
         <v>80</v>
       </c>
@@ -2662,12 +2555,12 @@
         <v>81</v>
       </c>
     </row>
-    <row r="79" spans="1:3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="81" spans="1:6" ht="28.5" customHeight="1">
+    <row r="81" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C81" s="11" t="s">
         <v>83</v>
       </c>
@@ -2681,7 +2574,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="82" spans="1:6" ht="50.1" customHeight="1">
+    <row r="82" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C82" s="9" t="s">
         <v>87</v>
       </c>
@@ -2695,7 +2588,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="50.1" customHeight="1">
+    <row r="83" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C83" s="9" t="s">
         <v>91</v>
       </c>
@@ -2709,7 +2602,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="84" spans="1:6" ht="50.1" customHeight="1">
+    <row r="84" spans="1:6" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C84" s="9" t="s">
         <v>95</v>
       </c>
@@ -2723,22 +2616,22 @@
         <v>98</v>
       </c>
     </row>
-    <row r="89" spans="1:6">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="91" spans="1:6">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B91" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="92" spans="1:6">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C92" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="93" spans="1:6">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C93" t="s">
         <v>102</v>
       </c>
@@ -2770,25 +2663,25 @@
       <selection activeCell="E68" sqref="E68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="2" max="2" width="16.1640625" customWidth="1"/>
     <col min="3" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="61.85546875" customWidth="1"/>
-    <col min="6" max="6" width="130.85546875" customWidth="1"/>
-    <col min="7" max="7" width="52.85546875" customWidth="1"/>
+    <col min="5" max="5" width="61.83203125" customWidth="1"/>
+    <col min="6" max="6" width="130.83203125" customWidth="1"/>
+    <col min="7" max="7" width="52.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C2" s="2" t="s">
         <v>103</v>
       </c>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="31"/>
     </row>
-    <row r="4" spans="1:6" ht="30.75" customHeight="1">
+    <row r="4" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="12" t="s">
         <v>104</v>
       </c>
@@ -2805,7 +2698,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="1" customFormat="1" ht="41.45">
+    <row r="5" spans="1:6" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A5" s="27" t="s">
         <v>69</v>
       </c>
@@ -2825,7 +2718,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="1" customFormat="1" ht="55.15">
+    <row r="6" spans="1:6" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="B6" s="28" t="s">
         <v>114</v>
       </c>
@@ -2842,7 +2735,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="1" customFormat="1" ht="55.15">
+    <row r="7" spans="1:6" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.2">
       <c r="B7" s="28" t="s">
         <v>119</v>
       </c>
@@ -2859,7 +2752,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="1" customFormat="1" ht="55.15">
+    <row r="8" spans="1:6" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="B8" s="28" t="s">
         <v>124</v>
       </c>
@@ -2876,7 +2769,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="1" customFormat="1" ht="43.5" customHeight="1">
+    <row r="9" spans="1:6" s="1" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="28" t="s">
         <v>129</v>
       </c>
@@ -2893,7 +2786,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="1" customFormat="1" ht="60" customHeight="1">
+    <row r="10" spans="1:6" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="28" t="s">
         <v>134</v>
       </c>
@@ -2910,7 +2803,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="1" customFormat="1" ht="43.5" customHeight="1">
+    <row r="11" spans="1:6" s="1" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="28" t="s">
         <v>138</v>
       </c>
@@ -2927,7 +2820,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="1" customFormat="1" ht="43.5" customHeight="1">
+    <row r="12" spans="1:6" s="1" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="28" t="s">
         <v>142</v>
       </c>
@@ -2944,7 +2837,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="1" customFormat="1" ht="56.25" customHeight="1">
+    <row r="13" spans="1:6" s="1" customFormat="1" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="28" t="s">
         <v>146</v>
       </c>
@@ -2961,7 +2854,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="1" customFormat="1" ht="77.25" customHeight="1">
+    <row r="14" spans="1:6" s="1" customFormat="1" ht="77.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="28" t="s">
         <v>149</v>
       </c>
@@ -2978,18 +2871,18 @@
         <v>153</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="1" customFormat="1" ht="15" customHeight="1"/>
-    <row r="16" spans="1:6" s="1" customFormat="1" ht="15" customHeight="1"/>
-    <row r="17" spans="1:6" ht="15" customHeight="1">
+    <row r="15" spans="1:6" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:6" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="1:6" ht="15" customHeight="1">
+    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="62.25" customHeight="1">
+    <row r="19" spans="1:6" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="17" t="s">
         <v>154</v>
       </c>
@@ -3004,67 +2897,67 @@
         <v>157</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15" customHeight="1">
-      <c r="B20" s="47" t="s">
+    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="44" t="s">
         <v>158</v>
       </c>
-      <c r="C20" s="49" t="s">
+      <c r="C20" s="46" t="s">
         <v>159</v>
       </c>
       <c r="D20" s="8"/>
-      <c r="E20" s="49" t="s">
+      <c r="E20" s="46" t="s">
         <v>160</v>
       </c>
-      <c r="F20" s="48"/>
-    </row>
-    <row r="21" spans="1:6" ht="15" customHeight="1">
-      <c r="B21" s="47"/>
-      <c r="C21" s="49"/>
+      <c r="F20" s="45"/>
+    </row>
+    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="44"/>
+      <c r="C21" s="46"/>
       <c r="D21" s="8"/>
-      <c r="E21" s="49"/>
-      <c r="F21" s="48"/>
-    </row>
-    <row r="22" spans="1:6" ht="15" customHeight="1">
-      <c r="B22" s="47" t="s">
+      <c r="E21" s="46"/>
+      <c r="F21" s="45"/>
+    </row>
+    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="44" t="s">
         <v>161</v>
       </c>
-      <c r="C22" s="49" t="s">
+      <c r="C22" s="46" t="s">
         <v>162</v>
       </c>
       <c r="D22" s="8"/>
-      <c r="E22" s="49" t="s">
+      <c r="E22" s="46" t="s">
         <v>163</v>
       </c>
-      <c r="F22" s="48"/>
-    </row>
-    <row r="23" spans="1:6" ht="15" customHeight="1">
-      <c r="B23" s="47"/>
-      <c r="C23" s="49"/>
+      <c r="F22" s="45"/>
+    </row>
+    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="44"/>
+      <c r="C23" s="46"/>
       <c r="D23" s="8"/>
-      <c r="E23" s="49"/>
-      <c r="F23" s="48"/>
-    </row>
-    <row r="24" spans="1:6" ht="15" customHeight="1">
-      <c r="B24" s="47" t="s">
+      <c r="E23" s="46"/>
+      <c r="F23" s="45"/>
+    </row>
+    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="44" t="s">
         <v>164</v>
       </c>
-      <c r="C24" s="49" t="s">
+      <c r="C24" s="46" t="s">
         <v>165</v>
       </c>
       <c r="D24" s="8"/>
-      <c r="E24" s="49" t="s">
+      <c r="E24" s="46" t="s">
         <v>166</v>
       </c>
-      <c r="F24" s="48"/>
-    </row>
-    <row r="25" spans="1:6" ht="15" customHeight="1">
-      <c r="B25" s="47"/>
-      <c r="C25" s="49"/>
+      <c r="F24" s="45"/>
+    </row>
+    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="44"/>
+      <c r="C25" s="46"/>
       <c r="D25" s="8"/>
-      <c r="E25" s="49"/>
-      <c r="F25" s="48"/>
-    </row>
-    <row r="26" spans="1:6" ht="30" customHeight="1">
+      <c r="E25" s="46"/>
+      <c r="F25" s="45"/>
+    </row>
+    <row r="26" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="20" t="s">
         <v>167</v>
       </c>
@@ -3077,7 +2970,7 @@
       </c>
       <c r="F26" s="21"/>
     </row>
-    <row r="27" spans="1:6" ht="30" customHeight="1">
+    <row r="27" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="22" t="s">
         <v>170</v>
       </c>
@@ -3090,7 +2983,7 @@
       </c>
       <c r="F27" s="21"/>
     </row>
-    <row r="28" spans="1:6" ht="30" customHeight="1">
+    <row r="28" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="20" t="s">
         <v>173</v>
       </c>
@@ -3103,7 +2996,7 @@
       </c>
       <c r="F28" s="21"/>
     </row>
-    <row r="29" spans="1:6" ht="30" customHeight="1">
+    <row r="29" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="20" t="s">
         <v>176</v>
       </c>
@@ -3116,7 +3009,7 @@
       </c>
       <c r="F29" s="21"/>
     </row>
-    <row r="30" spans="1:6" ht="30" customHeight="1">
+    <row r="30" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="20" t="s">
         <v>179</v>
       </c>
@@ -3129,291 +3022,291 @@
       </c>
       <c r="F30" s="21"/>
     </row>
-    <row r="31" spans="1:6" ht="15" customHeight="1">
-      <c r="B31" s="47" t="s">
+    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="C31" s="49" t="s">
+      <c r="C31" s="46" t="s">
         <v>183</v>
       </c>
       <c r="D31" s="8"/>
-      <c r="E31" s="49" t="s">
+      <c r="E31" s="46" t="s">
         <v>184</v>
       </c>
-      <c r="F31" s="48"/>
-    </row>
-    <row r="32" spans="1:6" ht="15" customHeight="1">
-      <c r="B32" s="47"/>
-      <c r="C32" s="49"/>
+      <c r="F31" s="45"/>
+    </row>
+    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B32" s="44"/>
+      <c r="C32" s="46"/>
       <c r="D32" s="8"/>
-      <c r="E32" s="49"/>
-      <c r="F32" s="48"/>
-    </row>
-    <row r="33" spans="2:6" ht="20.100000000000001" customHeight="1">
-      <c r="B33" s="47" t="s">
+      <c r="E32" s="46"/>
+      <c r="F32" s="45"/>
+    </row>
+    <row r="33" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="44" t="s">
         <v>185</v>
       </c>
-      <c r="C33" s="49" t="s">
+      <c r="C33" s="46" t="s">
         <v>186</v>
       </c>
       <c r="D33" s="8"/>
-      <c r="E33" s="49" t="s">
+      <c r="E33" s="46" t="s">
         <v>187</v>
       </c>
-      <c r="F33" s="48"/>
-    </row>
-    <row r="34" spans="2:6" ht="20.100000000000001" customHeight="1">
-      <c r="B34" s="47"/>
-      <c r="C34" s="49"/>
+      <c r="F33" s="45"/>
+    </row>
+    <row r="34" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="44"/>
+      <c r="C34" s="46"/>
       <c r="D34" s="8"/>
-      <c r="E34" s="49"/>
-      <c r="F34" s="48"/>
-    </row>
-    <row r="35" spans="2:6" ht="20.100000000000001" customHeight="1">
-      <c r="B35" s="47" t="s">
+      <c r="E34" s="46"/>
+      <c r="F34" s="45"/>
+    </row>
+    <row r="35" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B35" s="44" t="s">
         <v>188</v>
       </c>
-      <c r="C35" s="49" t="s">
+      <c r="C35" s="46" t="s">
         <v>189</v>
       </c>
       <c r="D35" s="8"/>
-      <c r="E35" s="49" t="s">
+      <c r="E35" s="46" t="s">
         <v>190</v>
       </c>
-      <c r="F35" s="48"/>
-    </row>
-    <row r="36" spans="2:6" ht="20.100000000000001" customHeight="1">
-      <c r="B36" s="47"/>
-      <c r="C36" s="49"/>
+      <c r="F35" s="45"/>
+    </row>
+    <row r="36" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B36" s="44"/>
+      <c r="C36" s="46"/>
       <c r="D36" s="8"/>
-      <c r="E36" s="49"/>
-      <c r="F36" s="48"/>
-    </row>
-    <row r="37" spans="2:6" ht="20.100000000000001" customHeight="1">
-      <c r="B37" s="47" t="s">
+      <c r="E36" s="46"/>
+      <c r="F36" s="45"/>
+    </row>
+    <row r="37" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B37" s="44" t="s">
         <v>191</v>
       </c>
-      <c r="C37" s="49" t="s">
+      <c r="C37" s="46" t="s">
         <v>192</v>
       </c>
       <c r="D37" s="8"/>
-      <c r="E37" s="49" t="s">
+      <c r="E37" s="46" t="s">
         <v>193</v>
       </c>
-      <c r="F37" s="48"/>
-    </row>
-    <row r="38" spans="2:6" ht="20.100000000000001" customHeight="1">
-      <c r="B38" s="47"/>
-      <c r="C38" s="49"/>
+      <c r="F37" s="45"/>
+    </row>
+    <row r="38" spans="2:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B38" s="44"/>
+      <c r="C38" s="46"/>
       <c r="D38" s="8"/>
-      <c r="E38" s="49"/>
-      <c r="F38" s="48"/>
-    </row>
-    <row r="39" spans="2:6" ht="15" customHeight="1">
-      <c r="B39" s="47" t="s">
+      <c r="E38" s="46"/>
+      <c r="F38" s="45"/>
+    </row>
+    <row r="39" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B39" s="44" t="s">
         <v>194</v>
       </c>
-      <c r="C39" s="49" t="s">
+      <c r="C39" s="46" t="s">
         <v>195</v>
       </c>
       <c r="D39" s="8"/>
-      <c r="E39" s="49" t="s">
+      <c r="E39" s="46" t="s">
         <v>196</v>
       </c>
-      <c r="F39" s="48"/>
-    </row>
-    <row r="40" spans="2:6" ht="15" customHeight="1">
-      <c r="B40" s="47"/>
-      <c r="C40" s="49"/>
+      <c r="F39" s="45"/>
+    </row>
+    <row r="40" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B40" s="44"/>
+      <c r="C40" s="46"/>
       <c r="D40" s="8"/>
-      <c r="E40" s="49"/>
-      <c r="F40" s="48"/>
-    </row>
-    <row r="41" spans="2:6" ht="15" customHeight="1">
-      <c r="B41" s="47" t="s">
+      <c r="E40" s="46"/>
+      <c r="F40" s="45"/>
+    </row>
+    <row r="41" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B41" s="44" t="s">
         <v>197</v>
       </c>
-      <c r="C41" s="49" t="s">
+      <c r="C41" s="46" t="s">
         <v>198</v>
       </c>
       <c r="D41" s="8"/>
-      <c r="E41" s="49" t="s">
+      <c r="E41" s="46" t="s">
         <v>199</v>
       </c>
-      <c r="F41" s="48"/>
-    </row>
-    <row r="42" spans="2:6" ht="15" customHeight="1">
-      <c r="B42" s="47"/>
-      <c r="C42" s="49"/>
+      <c r="F41" s="45"/>
+    </row>
+    <row r="42" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B42" s="44"/>
+      <c r="C42" s="46"/>
       <c r="D42" s="8"/>
-      <c r="E42" s="49"/>
-      <c r="F42" s="48"/>
-    </row>
-    <row r="43" spans="2:6" ht="21.95" customHeight="1">
-      <c r="B43" s="47" t="s">
+      <c r="E42" s="46"/>
+      <c r="F42" s="45"/>
+    </row>
+    <row r="43" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B43" s="44" t="s">
         <v>200</v>
       </c>
-      <c r="C43" s="49" t="s">
+      <c r="C43" s="46" t="s">
         <v>201</v>
       </c>
       <c r="D43" s="8"/>
-      <c r="E43" s="49" t="s">
+      <c r="E43" s="46" t="s">
         <v>202</v>
       </c>
-      <c r="F43" s="48"/>
-    </row>
-    <row r="44" spans="2:6" ht="21.95" customHeight="1">
-      <c r="B44" s="47"/>
-      <c r="C44" s="49"/>
+      <c r="F43" s="45"/>
+    </row>
+    <row r="44" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B44" s="44"/>
+      <c r="C44" s="46"/>
       <c r="D44" s="8"/>
-      <c r="E44" s="49"/>
-      <c r="F44" s="48"/>
-    </row>
-    <row r="45" spans="2:6" ht="21.95" customHeight="1">
-      <c r="B45" s="47" t="s">
+      <c r="E44" s="46"/>
+      <c r="F44" s="45"/>
+    </row>
+    <row r="45" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B45" s="44" t="s">
         <v>203</v>
       </c>
-      <c r="C45" s="49" t="s">
+      <c r="C45" s="46" t="s">
         <v>204</v>
       </c>
       <c r="D45" s="8"/>
-      <c r="E45" s="49" t="s">
+      <c r="E45" s="46" t="s">
         <v>205</v>
       </c>
-      <c r="F45" s="48"/>
-    </row>
-    <row r="46" spans="2:6" ht="21.95" customHeight="1">
-      <c r="B46" s="47"/>
-      <c r="C46" s="49"/>
+      <c r="F45" s="45"/>
+    </row>
+    <row r="46" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B46" s="44"/>
+      <c r="C46" s="46"/>
       <c r="D46" s="8"/>
-      <c r="E46" s="49"/>
-      <c r="F46" s="48"/>
-    </row>
-    <row r="47" spans="2:6" ht="21.95" customHeight="1">
-      <c r="B47" s="47" t="s">
+      <c r="E46" s="46"/>
+      <c r="F46" s="45"/>
+    </row>
+    <row r="47" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B47" s="44" t="s">
         <v>206</v>
       </c>
-      <c r="C47" s="49" t="s">
+      <c r="C47" s="46" t="s">
         <v>207</v>
       </c>
       <c r="D47" s="8"/>
-      <c r="E47" s="49" t="s">
+      <c r="E47" s="46" t="s">
         <v>208</v>
       </c>
-      <c r="F47" s="48"/>
-    </row>
-    <row r="48" spans="2:6" ht="21.95" customHeight="1">
-      <c r="B48" s="47"/>
-      <c r="C48" s="49"/>
+      <c r="F47" s="45"/>
+    </row>
+    <row r="48" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B48" s="44"/>
+      <c r="C48" s="46"/>
       <c r="D48" s="8"/>
-      <c r="E48" s="49"/>
-      <c r="F48" s="48"/>
-    </row>
-    <row r="49" spans="2:6" ht="21.95" customHeight="1">
-      <c r="B49" s="47" t="s">
+      <c r="E48" s="46"/>
+      <c r="F48" s="45"/>
+    </row>
+    <row r="49" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B49" s="44" t="s">
         <v>209</v>
       </c>
-      <c r="C49" s="49" t="s">
+      <c r="C49" s="46" t="s">
         <v>210</v>
       </c>
       <c r="D49" s="8"/>
-      <c r="E49" s="49" t="s">
+      <c r="E49" s="46" t="s">
         <v>211</v>
       </c>
-      <c r="F49" s="48" t="s">
+      <c r="F49" s="45" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="50" spans="2:6" ht="69.75" customHeight="1">
-      <c r="B50" s="47"/>
-      <c r="C50" s="49"/>
+    <row r="50" spans="2:6" ht="69.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B50" s="44"/>
+      <c r="C50" s="46"/>
       <c r="D50" s="8"/>
-      <c r="E50" s="49"/>
-      <c r="F50" s="48"/>
-    </row>
-    <row r="51" spans="2:6" ht="21.95" customHeight="1">
-      <c r="B51" s="47" t="s">
+      <c r="E50" s="46"/>
+      <c r="F50" s="45"/>
+    </row>
+    <row r="51" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B51" s="44" t="s">
         <v>213</v>
       </c>
-      <c r="C51" s="49" t="s">
+      <c r="C51" s="46" t="s">
         <v>214</v>
       </c>
       <c r="D51" s="8"/>
-      <c r="E51" s="49" t="s">
+      <c r="E51" s="46" t="s">
         <v>215</v>
       </c>
-      <c r="F51" s="48" t="s">
+      <c r="F51" s="45" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="52" spans="2:6" ht="21.95" customHeight="1">
-      <c r="B52" s="47"/>
-      <c r="C52" s="49"/>
+    <row r="52" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B52" s="44"/>
+      <c r="C52" s="46"/>
       <c r="D52" s="8"/>
-      <c r="E52" s="49"/>
-      <c r="F52" s="48"/>
-    </row>
-    <row r="53" spans="2:6" ht="21.95" customHeight="1">
-      <c r="B53" s="47" t="s">
+      <c r="E52" s="46"/>
+      <c r="F52" s="45"/>
+    </row>
+    <row r="53" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B53" s="44" t="s">
         <v>217</v>
       </c>
-      <c r="C53" s="49" t="s">
+      <c r="C53" s="46" t="s">
         <v>218</v>
       </c>
       <c r="D53" s="8"/>
-      <c r="E53" s="49" t="s">
+      <c r="E53" s="46" t="s">
         <v>219</v>
       </c>
-      <c r="F53" s="48"/>
-    </row>
-    <row r="54" spans="2:6" ht="21.95" customHeight="1">
-      <c r="B54" s="47"/>
-      <c r="C54" s="49"/>
+      <c r="F53" s="45"/>
+    </row>
+    <row r="54" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B54" s="44"/>
+      <c r="C54" s="46"/>
       <c r="D54" s="8"/>
-      <c r="E54" s="49"/>
-      <c r="F54" s="48"/>
-    </row>
-    <row r="55" spans="2:6" ht="15" customHeight="1">
-      <c r="B55" s="47" t="s">
+      <c r="E54" s="46"/>
+      <c r="F54" s="45"/>
+    </row>
+    <row r="55" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B55" s="44" t="s">
         <v>220</v>
       </c>
-      <c r="C55" s="49" t="s">
+      <c r="C55" s="46" t="s">
         <v>221</v>
       </c>
       <c r="D55" s="8"/>
-      <c r="E55" s="49" t="s">
+      <c r="E55" s="46" t="s">
         <v>222</v>
       </c>
-      <c r="F55" s="48"/>
-    </row>
-    <row r="56" spans="2:6" ht="15" customHeight="1">
-      <c r="B56" s="47"/>
-      <c r="C56" s="49"/>
+      <c r="F55" s="45"/>
+    </row>
+    <row r="56" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B56" s="44"/>
+      <c r="C56" s="46"/>
       <c r="D56" s="8"/>
-      <c r="E56" s="49"/>
-      <c r="F56" s="48"/>
-    </row>
-    <row r="57" spans="2:6" ht="15" customHeight="1">
-      <c r="B57" s="47" t="s">
+      <c r="E56" s="46"/>
+      <c r="F56" s="45"/>
+    </row>
+    <row r="57" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B57" s="44" t="s">
         <v>223</v>
       </c>
-      <c r="C57" s="49" t="s">
+      <c r="C57" s="46" t="s">
         <v>224</v>
       </c>
       <c r="D57" s="8"/>
-      <c r="E57" s="49" t="s">
+      <c r="E57" s="46" t="s">
         <v>225</v>
       </c>
-      <c r="F57" s="48"/>
-    </row>
-    <row r="58" spans="2:6" ht="15" customHeight="1">
-      <c r="B58" s="47"/>
-      <c r="C58" s="49"/>
+      <c r="F57" s="45"/>
+    </row>
+    <row r="58" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B58" s="44"/>
+      <c r="C58" s="46"/>
       <c r="D58" s="8"/>
-      <c r="E58" s="49"/>
-      <c r="F58" s="48"/>
-    </row>
-    <row r="59" spans="2:6" ht="52.9">
+      <c r="E58" s="46"/>
+      <c r="F58" s="45"/>
+    </row>
+    <row r="59" spans="2:6" ht="56" x14ac:dyDescent="0.2">
       <c r="B59" s="20" t="s">
         <v>226</v>
       </c>
@@ -3428,147 +3321,147 @@
         <v>229</v>
       </c>
     </row>
-    <row r="60" spans="2:6" ht="21.95" customHeight="1">
-      <c r="B60" s="47" t="s">
+    <row r="60" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B60" s="44" t="s">
         <v>230</v>
       </c>
-      <c r="C60" s="49" t="s">
+      <c r="C60" s="46" t="s">
         <v>231</v>
       </c>
       <c r="D60" s="8"/>
-      <c r="E60" s="49" t="s">
+      <c r="E60" s="46" t="s">
         <v>232</v>
       </c>
-      <c r="F60" s="48"/>
-    </row>
-    <row r="61" spans="2:6" ht="21.95" customHeight="1">
-      <c r="B61" s="47"/>
-      <c r="C61" s="49"/>
+      <c r="F60" s="45"/>
+    </row>
+    <row r="61" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B61" s="44"/>
+      <c r="C61" s="46"/>
       <c r="D61" s="8"/>
-      <c r="E61" s="49"/>
-      <c r="F61" s="48"/>
-    </row>
-    <row r="62" spans="2:6" ht="21.95" customHeight="1">
-      <c r="B62" s="47" t="s">
+      <c r="E61" s="46"/>
+      <c r="F61" s="45"/>
+    </row>
+    <row r="62" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B62" s="44" t="s">
         <v>233</v>
       </c>
-      <c r="C62" s="49" t="s">
+      <c r="C62" s="46" t="s">
         <v>234</v>
       </c>
       <c r="D62" s="8"/>
-      <c r="E62" s="49" t="s">
+      <c r="E62" s="46" t="s">
         <v>235</v>
       </c>
-      <c r="F62" s="48"/>
-    </row>
-    <row r="63" spans="2:6" ht="21.95" customHeight="1">
-      <c r="B63" s="47"/>
-      <c r="C63" s="49"/>
+      <c r="F62" s="45"/>
+    </row>
+    <row r="63" spans="2:6" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B63" s="44"/>
+      <c r="C63" s="46"/>
       <c r="D63" s="8"/>
-      <c r="E63" s="49"/>
-      <c r="F63" s="48"/>
-    </row>
-    <row r="64" spans="2:6" ht="15" customHeight="1">
-      <c r="B64" s="47" t="s">
+      <c r="E63" s="46"/>
+      <c r="F63" s="45"/>
+    </row>
+    <row r="64" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B64" s="44" t="s">
         <v>236</v>
       </c>
-      <c r="C64" s="49" t="s">
+      <c r="C64" s="46" t="s">
         <v>237</v>
       </c>
       <c r="D64" s="8"/>
-      <c r="E64" s="49" t="s">
+      <c r="E64" s="46" t="s">
         <v>238</v>
       </c>
-      <c r="F64" s="48"/>
-    </row>
-    <row r="65" spans="1:6" ht="15" customHeight="1">
-      <c r="B65" s="47"/>
-      <c r="C65" s="49"/>
+      <c r="F64" s="45"/>
+    </row>
+    <row r="65" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B65" s="44"/>
+      <c r="C65" s="46"/>
       <c r="D65" s="8"/>
-      <c r="E65" s="49"/>
-      <c r="F65" s="48"/>
-    </row>
-    <row r="66" spans="1:6" ht="15" customHeight="1">
-      <c r="B66" s="47" t="s">
+      <c r="E65" s="46"/>
+      <c r="F65" s="45"/>
+    </row>
+    <row r="66" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B66" s="44" t="s">
         <v>239</v>
       </c>
-      <c r="C66" s="49" t="s">
+      <c r="C66" s="46" t="s">
         <v>240</v>
       </c>
       <c r="D66" s="8"/>
-      <c r="E66" s="49" t="s">
+      <c r="E66" s="46" t="s">
         <v>241</v>
       </c>
-      <c r="F66" s="48"/>
-    </row>
-    <row r="67" spans="1:6" ht="15" customHeight="1">
-      <c r="B67" s="47"/>
-      <c r="C67" s="49"/>
+      <c r="F66" s="45"/>
+    </row>
+    <row r="67" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B67" s="44"/>
+      <c r="C67" s="46"/>
       <c r="D67" s="8"/>
-      <c r="E67" s="49"/>
-      <c r="F67" s="48"/>
-    </row>
-    <row r="68" spans="1:6" ht="15" customHeight="1">
-      <c r="B68" s="47" t="s">
+      <c r="E67" s="46"/>
+      <c r="F67" s="45"/>
+    </row>
+    <row r="68" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B68" s="44" t="s">
         <v>242</v>
       </c>
-      <c r="C68" s="49" t="s">
+      <c r="C68" s="46" t="s">
         <v>243</v>
       </c>
       <c r="D68" s="8"/>
-      <c r="E68" s="49" t="s">
+      <c r="E68" s="46" t="s">
         <v>244</v>
       </c>
-      <c r="F68" s="48"/>
-    </row>
-    <row r="69" spans="1:6" ht="15" customHeight="1">
-      <c r="B69" s="47"/>
-      <c r="C69" s="49"/>
+      <c r="F68" s="45"/>
+    </row>
+    <row r="69" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B69" s="44"/>
+      <c r="C69" s="46"/>
       <c r="D69" s="8"/>
-      <c r="E69" s="49"/>
-      <c r="F69" s="48"/>
-    </row>
-    <row r="70" spans="1:6" ht="15" customHeight="1">
-      <c r="B70" s="47" t="s">
+      <c r="E69" s="46"/>
+      <c r="F69" s="45"/>
+    </row>
+    <row r="70" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B70" s="44" t="s">
         <v>245</v>
       </c>
-      <c r="C70" s="49" t="s">
+      <c r="C70" s="46" t="s">
         <v>246</v>
       </c>
       <c r="D70" s="8"/>
-      <c r="E70" s="49" t="s">
+      <c r="E70" s="46" t="s">
         <v>244</v>
       </c>
-      <c r="F70" s="48"/>
-    </row>
-    <row r="71" spans="1:6" ht="15" customHeight="1">
-      <c r="B71" s="47"/>
-      <c r="C71" s="49"/>
+      <c r="F70" s="45"/>
+    </row>
+    <row r="71" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B71" s="44"/>
+      <c r="C71" s="46"/>
       <c r="D71" s="8"/>
-      <c r="E71" s="49"/>
-      <c r="F71" s="48"/>
-    </row>
-    <row r="72" spans="1:6" ht="15" customHeight="1">
-      <c r="B72" s="47" t="s">
+      <c r="E71" s="46"/>
+      <c r="F71" s="45"/>
+    </row>
+    <row r="72" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B72" s="44" t="s">
         <v>247</v>
       </c>
-      <c r="C72" s="49" t="s">
+      <c r="C72" s="46" t="s">
         <v>248</v>
       </c>
       <c r="D72" s="8"/>
-      <c r="E72" s="49" t="s">
+      <c r="E72" s="46" t="s">
         <v>249</v>
       </c>
-      <c r="F72" s="48"/>
-    </row>
-    <row r="73" spans="1:6" ht="15" customHeight="1">
-      <c r="B73" s="47"/>
-      <c r="C73" s="49"/>
+      <c r="F72" s="45"/>
+    </row>
+    <row r="73" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B73" s="44"/>
+      <c r="C73" s="46"/>
       <c r="D73" s="8"/>
-      <c r="E73" s="49"/>
-      <c r="F73" s="48"/>
-    </row>
-    <row r="74" spans="1:6" ht="39" customHeight="1">
+      <c r="E73" s="46"/>
+      <c r="F73" s="45"/>
+    </row>
+    <row r="74" spans="1:6" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B74" s="23" t="s">
         <v>250</v>
       </c>
@@ -3581,29 +3474,29 @@
       </c>
       <c r="F74" s="25"/>
     </row>
-    <row r="75" spans="1:6">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B75" s="7"/>
     </row>
-    <row r="76" spans="1:6" ht="15" customHeight="1"/>
-    <row r="77" spans="1:6" ht="15" customHeight="1"/>
-    <row r="78" spans="1:6" ht="15" customHeight="1"/>
-    <row r="79" spans="1:6" ht="15" customHeight="1">
+    <row r="76" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="77" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="78" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="79" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="15" customHeight="1"/>
-    <row r="81" spans="1:6" ht="15" customHeight="1"/>
-    <row r="82" spans="1:6" ht="15" customHeight="1"/>
-    <row r="83" spans="1:6" ht="15" customHeight="1"/>
-    <row r="84" spans="1:6" ht="15" customHeight="1"/>
-    <row r="85" spans="1:6" ht="15" customHeight="1"/>
-    <row r="86" spans="1:6" ht="15" customHeight="1">
+    <row r="80" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="81" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="82" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="83" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="84" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="85" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="86" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="89" spans="1:6" ht="55.15">
+    <row r="89" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="B89" s="28" t="s">
         <v>252</v>
       </c>
@@ -3620,7 +3513,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="90" spans="1:6" ht="55.15">
+    <row r="90" spans="1:6" ht="60" x14ac:dyDescent="0.2">
       <c r="B90" s="28" t="s">
         <v>253</v>
       </c>
@@ -3637,7 +3530,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="91" spans="1:6" ht="55.15">
+    <row r="91" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="B91" s="28" t="s">
         <v>254</v>
       </c>
@@ -3654,7 +3547,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="92" spans="1:6" ht="27.6">
+    <row r="92" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="B92" s="28" t="s">
         <v>255</v>
       </c>
@@ -3671,7 +3564,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="93" spans="1:6" ht="41.45">
+    <row r="93" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="B93" s="28" t="s">
         <v>256</v>
       </c>
@@ -3688,7 +3581,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="94" spans="1:6" ht="89.25" customHeight="1">
+    <row r="94" spans="1:6" ht="89.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B94" s="28" t="s">
         <v>257</v>
       </c>
@@ -3705,7 +3598,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="95" spans="1:6" ht="63" customHeight="1">
+    <row r="95" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B95" s="28" t="s">
         <v>260</v>
       </c>
@@ -3829,32 +3722,32 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65E1B3F2-147D-4DA9-9642-3C715D567C87}">
-  <dimension ref="B1:V33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65E1B3F2-147D-4DA9-9642-3C715D567C87}">
+  <dimension ref="B1:V28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="16"/>
-    <col min="2" max="2" width="30.5703125" style="16" customWidth="1"/>
-    <col min="3" max="3" width="54.5703125" style="16" customWidth="1"/>
-    <col min="4" max="4" width="38.5703125" style="16" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" style="16"/>
+    <col min="2" max="2" width="32.83203125" style="16" customWidth="1"/>
+    <col min="3" max="3" width="54.5" style="16" customWidth="1"/>
+    <col min="4" max="4" width="38.5" style="16" customWidth="1"/>
     <col min="5" max="5" width="45" style="16" customWidth="1"/>
-    <col min="6" max="6" width="33.140625" style="16" customWidth="1"/>
-    <col min="7" max="7" width="58.7109375" style="16" customWidth="1"/>
-    <col min="8" max="22" width="12.7109375" style="16" customWidth="1"/>
-    <col min="23" max="16384" width="9.140625" style="16"/>
+    <col min="6" max="6" width="33.1640625" style="16" customWidth="1"/>
+    <col min="7" max="7" width="58.6640625" style="16" customWidth="1"/>
+    <col min="8" max="22" width="12.6640625" style="16" customWidth="1"/>
+    <col min="23" max="16384" width="9.1640625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:22">
-      <c r="B1" s="37" t="s">
+    <row r="1" spans="2:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="B1" s="35" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="4" spans="2:22" ht="27.75" customHeight="1">
+    <row r="4" spans="2:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="5" t="s">
         <v>264</v>
       </c>
@@ -3873,364 +3766,311 @@
       <c r="G4" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="H4" s="50" t="s">
+      <c r="H4" s="47" t="s">
         <v>268</v>
       </c>
-      <c r="I4" s="51"/>
-      <c r="J4" s="51"/>
-      <c r="K4" s="51"/>
-      <c r="L4" s="51"/>
-      <c r="M4" s="51"/>
-      <c r="N4" s="51"/>
-      <c r="O4" s="51"/>
-      <c r="P4" s="51"/>
-      <c r="Q4" s="51"/>
-      <c r="R4" s="51"/>
-      <c r="S4" s="51"/>
-      <c r="T4" s="51"/>
-      <c r="U4" s="51"/>
-      <c r="V4" s="51"/>
-    </row>
-    <row r="5" spans="2:22">
-      <c r="H5" s="40" t="s">
+      <c r="I4" s="48"/>
+      <c r="J4" s="48"/>
+      <c r="K4" s="48"/>
+      <c r="L4" s="48"/>
+      <c r="M4" s="48"/>
+      <c r="N4" s="48"/>
+      <c r="O4" s="48"/>
+      <c r="P4" s="48"/>
+      <c r="Q4" s="48"/>
+      <c r="R4" s="48"/>
+      <c r="S4" s="48"/>
+      <c r="T4" s="48"/>
+      <c r="U4" s="48"/>
+      <c r="V4" s="48"/>
+    </row>
+    <row r="5" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="H5" s="37" t="s">
         <v>269</v>
       </c>
-      <c r="I5" s="40" t="s">
+      <c r="I5" s="37" t="s">
         <v>270</v>
       </c>
-      <c r="J5" s="40" t="s">
+      <c r="J5" s="37" t="s">
         <v>271</v>
       </c>
-      <c r="K5" s="40" t="s">
+      <c r="K5" s="37" t="s">
         <v>272</v>
       </c>
-      <c r="L5" s="40" t="s">
+      <c r="L5" s="37" t="s">
         <v>273</v>
       </c>
-      <c r="M5" s="40" t="s">
+      <c r="M5" s="37" t="s">
         <v>274</v>
       </c>
-      <c r="N5" s="40" t="s">
+      <c r="N5" s="37" t="s">
         <v>275</v>
       </c>
-      <c r="O5" s="40" t="s">
+      <c r="O5" s="37" t="s">
         <v>276</v>
       </c>
-      <c r="P5" s="40" t="s">
+      <c r="P5" s="37" t="s">
         <v>277</v>
       </c>
-      <c r="Q5" s="40" t="s">
+      <c r="Q5" s="37" t="s">
         <v>278</v>
       </c>
-      <c r="R5" s="40" t="s">
+      <c r="R5" s="37" t="s">
         <v>279</v>
       </c>
-      <c r="S5" s="40" t="s">
+      <c r="S5" s="37" t="s">
         <v>280</v>
       </c>
-      <c r="T5" s="40" t="s">
+      <c r="T5" s="37" t="s">
         <v>281</v>
       </c>
-      <c r="U5" s="40" t="s">
+      <c r="U5" s="37" t="s">
         <v>282</v>
       </c>
-      <c r="V5" s="40" t="s">
+      <c r="V5" s="37" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="6" spans="2:22">
-      <c r="B6" s="41" t="s">
+    <row r="6" spans="2:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="B6" s="38" t="s">
         <v>284</v>
       </c>
-      <c r="C6" s="35" t="s">
+      <c r="C6" s="33"/>
+    </row>
+    <row r="7" spans="2:22" ht="32" x14ac:dyDescent="0.2">
+      <c r="B7" s="16" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="7" spans="2:22" ht="43.15">
-      <c r="B7" s="16" t="s">
+      <c r="C7" s="16" t="s">
         <v>286</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="D7" s="16" t="s">
         <v>287</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="E7" s="16" t="s">
         <v>288</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="F7" s="16" t="s">
         <v>289</v>
       </c>
-      <c r="F7" s="16" t="s">
+    </row>
+    <row r="8" spans="2:22" ht="48" x14ac:dyDescent="0.2">
+      <c r="B8" s="16" t="s">
         <v>290</v>
       </c>
-      <c r="G7" s="16" t="s">
+      <c r="C8" s="16" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="8" spans="2:22" ht="43.15">
-      <c r="B8" s="16" t="s">
+      <c r="D8" s="16" t="s">
         <v>292</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="E8" s="16" t="s">
         <v>293</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="F8" s="16" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="10" spans="2:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="B10" s="38" t="s">
         <v>294</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="C10" s="33"/>
+    </row>
+    <row r="11" spans="2:22" ht="48" x14ac:dyDescent="0.2">
+      <c r="B11" s="16" t="s">
         <v>295</v>
       </c>
-      <c r="F8" s="16" t="s">
-        <v>290</v>
-      </c>
-      <c r="G8" s="16" t="s">
+      <c r="C11" s="16" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="10" spans="2:22">
-      <c r="B10" s="41" t="s">
+      <c r="D11" s="16" t="s">
         <v>297</v>
       </c>
-      <c r="C10" s="35" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="11" spans="2:22" ht="72">
-      <c r="B11" s="16" t="s">
+      <c r="E11" s="16" t="s">
         <v>298</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="F11" s="16" t="s">
         <v>299</v>
       </c>
-      <c r="D11" s="16" t="s">
+    </row>
+    <row r="12" spans="2:22" ht="32" x14ac:dyDescent="0.2">
+      <c r="B12" s="16" t="s">
         <v>300</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="C12" s="16" t="s">
         <v>301</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="D12" s="16" t="s">
+        <v>333</v>
+      </c>
+      <c r="E12" s="16" t="s">
         <v>302</v>
       </c>
-      <c r="G11" s="16" t="s">
+      <c r="F12" s="16" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="12" spans="2:22" ht="28.9">
-      <c r="B12" s="16" t="s">
+    <row r="14" spans="2:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="B14" s="38" t="s">
         <v>304</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C14" s="33"/>
+    </row>
+    <row r="15" spans="2:22" ht="32" x14ac:dyDescent="0.2">
+      <c r="B15" s="16" t="s">
+        <v>337</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>338</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>340</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>339</v>
+      </c>
+      <c r="F15" s="16" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="16" spans="2:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="B16" s="16" t="s">
         <v>305</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="C16" s="16" t="s">
         <v>306</v>
       </c>
-      <c r="E12" s="16" t="s">
+      <c r="D16" s="16" t="s">
         <v>307</v>
       </c>
-      <c r="F12" s="16" t="s">
+      <c r="E16" s="16" t="s">
         <v>308</v>
       </c>
-      <c r="G12" s="16" t="s">
+      <c r="F16" s="16" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="14" spans="2:22" ht="28.9">
-      <c r="B14" s="41" t="s">
+    <row r="18" spans="2:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="B18" s="39" t="s">
         <v>310</v>
       </c>
-      <c r="C14" s="35" t="s">
+      <c r="C18" s="33"/>
+    </row>
+    <row r="19" spans="2:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="B19" s="16" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="15" spans="2:22" ht="28.9">
-      <c r="B15" s="16" t="s">
+      <c r="C19" s="16" t="s">
         <v>312</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="D19" s="16" t="s">
         <v>313</v>
       </c>
-      <c r="D15" s="16" t="s">
+      <c r="E19" s="16" t="s">
         <v>314</v>
       </c>
-      <c r="E15" s="16" t="s">
+      <c r="F19" s="16" t="s">
         <v>315</v>
       </c>
-      <c r="F15" s="16" t="s">
+    </row>
+    <row r="20" spans="2:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="B20" s="16" t="s">
         <v>316</v>
       </c>
-      <c r="G15" s="16" t="s">
+      <c r="C20" s="16" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="16" spans="2:22" ht="28.9">
-      <c r="B16" s="33" t="s">
+      <c r="D20" s="16" t="s">
+        <v>313</v>
+      </c>
+      <c r="E20" s="16" t="s">
+        <v>314</v>
+      </c>
+      <c r="F20" s="16" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="B21" s="16" t="s">
         <v>318</v>
       </c>
-      <c r="C16" s="33" t="s">
+      <c r="C21" s="16" t="s">
         <v>319</v>
       </c>
-      <c r="D16" s="33" t="s">
+      <c r="D21" s="16" t="s">
         <v>320</v>
       </c>
-      <c r="E16" s="33"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="42" t="s">
+      <c r="E21" s="16" t="s">
+        <v>314</v>
+      </c>
+      <c r="F21" s="16" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="17" spans="2:7">
-      <c r="B17" s="16" t="s">
+    <row r="22" spans="2:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="B22" s="16" t="s">
         <v>322</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="C22" s="16" t="s">
         <v>323</v>
       </c>
-      <c r="D17" s="16" t="s">
+      <c r="D22" s="16" t="s">
+        <v>320</v>
+      </c>
+      <c r="E22" s="16" t="s">
+        <v>314</v>
+      </c>
+      <c r="F22" s="16" t="s">
         <v>324</v>
       </c>
-      <c r="E17" s="16" t="s">
+    </row>
+    <row r="24" spans="2:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="B24" s="38" t="s">
         <v>325</v>
       </c>
-      <c r="F17" s="16" t="s">
+      <c r="C24" s="33"/>
+    </row>
+    <row r="25" spans="2:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="B25" s="16" t="s">
+        <v>335</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>334</v>
+      </c>
+      <c r="D25" s="16" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="19" spans="2:7" ht="28.9">
-      <c r="B19" s="34" t="s">
+      <c r="E25" s="16" t="s">
         <v>327</v>
       </c>
-      <c r="C19" s="35" t="s">
+      <c r="F25" s="16" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="B27" s="40" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="20" spans="2:7" ht="28.9">
-      <c r="B20" s="16" t="s">
+      <c r="C27" s="34"/>
+    </row>
+    <row r="28" spans="2:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="B28" s="16" t="s">
+        <v>336</v>
+      </c>
+      <c r="C28" s="16" t="s">
         <v>329</v>
       </c>
-      <c r="C20" s="16" t="s">
+      <c r="D28" s="36" t="s">
         <v>330</v>
       </c>
-      <c r="D20" s="16" t="s">
+      <c r="E28" s="16" t="s">
         <v>331</v>
       </c>
-      <c r="E20" s="16" t="s">
+      <c r="F28" s="16" t="s">
         <v>332</v>
       </c>
-      <c r="F20" s="16" t="s">
-        <v>333</v>
-      </c>
-      <c r="G20" s="16" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7">
-      <c r="B21" s="16" t="s">
-        <v>335</v>
-      </c>
-      <c r="C21" s="16" t="s">
-        <v>336</v>
-      </c>
-      <c r="D21" s="16" t="s">
-        <v>331</v>
-      </c>
-      <c r="E21" s="16" t="s">
-        <v>332</v>
-      </c>
-      <c r="F21" s="16" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7">
-      <c r="B22" s="16" t="s">
-        <v>337</v>
-      </c>
-      <c r="C22" s="16" t="s">
-        <v>338</v>
-      </c>
-      <c r="D22" s="16" t="s">
-        <v>339</v>
-      </c>
-      <c r="E22" s="16" t="s">
-        <v>332</v>
-      </c>
-      <c r="F22" s="16" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7">
-      <c r="B23" s="16" t="s">
-        <v>341</v>
-      </c>
-      <c r="C23" s="16" t="s">
-        <v>342</v>
-      </c>
-      <c r="D23" s="16" t="s">
-        <v>339</v>
-      </c>
-      <c r="E23" s="16" t="s">
-        <v>332</v>
-      </c>
-      <c r="F23" s="16" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7" ht="28.9">
-      <c r="B25" s="41" t="s">
-        <v>344</v>
-      </c>
-      <c r="C25" s="35" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" ht="28.9">
-      <c r="B26" s="16" t="s">
-        <v>346</v>
-      </c>
-      <c r="C26" s="16" t="s">
-        <v>347</v>
-      </c>
-      <c r="D26" s="16" t="s">
-        <v>348</v>
-      </c>
-      <c r="E26" s="16" t="s">
-        <v>349</v>
-      </c>
-      <c r="F26" s="16" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7" ht="28.9">
-      <c r="B28" s="38" t="s">
-        <v>351</v>
-      </c>
-      <c r="C28" s="36" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7" ht="57.6">
-      <c r="B29" s="16" t="s">
-        <v>353</v>
-      </c>
-      <c r="C29" s="16" t="s">
-        <v>354</v>
-      </c>
-      <c r="D29" s="39" t="s">
-        <v>355</v>
-      </c>
-      <c r="E29" s="36" t="s">
-        <v>356</v>
-      </c>
-      <c r="F29" s="36" t="s">
-        <v>357</v>
-      </c>
-      <c r="G29" s="36" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="33" spans="2:2" ht="28.9">
-      <c r="B33" s="43" t="s">
-        <v>359</v>
-      </c>
+      <c r="G28" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4241,20 +4081,10 @@
   <headerFooter>
     <oddHeader>&amp;C&amp;"Calibri"&amp;10&amp;K000000 Diffusione Limitata&amp;1#_x000D_</oddHeader>
   </headerFooter>
-  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010037C996546B721047AC306210F56DFE76" ma:contentTypeVersion="16" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="7019be02e39974b7d7220012a4395f64">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cebb5a04-f4fa-45b5-bfc7-4f29c5a77083" xmlns:ns3="5e884b80-f82b-4487-bc76-a4f46140e91f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="acf49b158ff560433ce502b7605146e2" ns2:_="" ns3:_="">
     <xsd:import namespace="cebb5a04-f4fa-45b5-bfc7-4f29c5a77083"/>
@@ -4495,7 +4325,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="5e884b80-f82b-4487-bc76-a4f46140e91f" xsi:nil="true"/>
@@ -4506,14 +4336,55 @@
 </p:properties>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{850ED4EC-3A53-4BA0-A0B2-ACB4E4BC6A85}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C70BC9A5-ED0E-44CF-87AB-439633C42FB9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="cebb5a04-f4fa-45b5-bfc7-4f29c5a77083"/>
+    <ds:schemaRef ds:uri="5e884b80-f82b-4487-bc76-a4f46140e91f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C70BC9A5-ED0E-44CF-87AB-439633C42FB9}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C6656D5-E04A-4314-A26F-C8902301C412}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5e884b80-f82b-4487-bc76-a4f46140e91f"/>
+    <ds:schemaRef ds:uri="cebb5a04-f4fa-45b5-bfc7-4f29c5a77083"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C6656D5-E04A-4314-A26F-C8902301C412}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{850ED4EC-3A53-4BA0-A0B2-ACB4E4BC6A85}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{0cf7ac0a-4681-4823-ab0b-04ef02c5f873}" enabled="1" method="Standard" siteId="{42f7676c-f455-423c-82f6-dc2d99791af7}" contentBits="0" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>